<commit_message>
update in end to end testing files
</commit_message>
<xml_diff>
--- a/end_to_end_testing.xlsx
+++ b/end_to_end_testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University_Study\Final Year Project\FYP-2\Project\TourToPK-Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E0D062-CA5F-403D-94B2-BC33E35F2995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2056A2EF-5D82-40AB-867F-1071A1B18499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FC72E4DC-F9F4-4E7B-B984-AE772E810068}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -229,13 +229,50 @@
 dashboard</t>
   </si>
   <si>
-    <t>admin  view, and deletes a details of places, recommended plan, hotels, and packages. Able to view and delete users</t>
-  </si>
-  <si>
     <t>hotel manager creates, edits, view, and deletes a details of hotels. Able to view and delete booking</t>
   </si>
   <si>
     <t>tour operator creates, edits, view, and deletes a details of packages .</t>
+  </si>
+  <si>
+    <t>1. go to the login page
+2. enter the valid data to log in
+3. able to create a new place
+4. able to view and delete place
+5. able to create a new plan
+6. able to view and delete plan
+7. able to view and delete preference
+8. logout.</t>
+  </si>
+  <si>
+    <t>admin  view, and deletes a details of places, recommended plan, hotels, and packages. Able to view and delete users and partner</t>
+  </si>
+  <si>
+    <t>1. go to the login page
+2. enter the valid data to log in
+3. able to view and delete place
+4. able to view and delete packages
+5. able to view and delete plan
+6. able to view and delete hotels
+7. able to view and delete users 
+8. logout.</t>
+  </si>
+  <si>
+    <t>1. go to the login page
+2. enter the valid data to log in
+3. able to create a new room
+4.able to update its profile
+5. able to view and delete hotels
+6. able to view and delete booking 
+7. logout.</t>
+  </si>
+  <si>
+    <t>1. go to the login page
+2. enter the valid data to log in
+3. able to create a new packages
+4. able to update its profile
+5. able to view and delete packages
+6. logout.</t>
   </si>
 </sst>
 </file>
@@ -627,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97996BF4-7082-4C7C-9347-F9A50C3056D2}">
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +831,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -804,11 +841,14 @@
       <c r="C11" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -816,13 +856,16 @@
         <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="E12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -830,13 +873,16 @@
         <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -844,7 +890,10 @@
         <v>46</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="E14" t="s">
         <v>19</v>

</xml_diff>